<commit_message>
Some work on the attitude controller and Phoenix Script
</commit_message>
<xml_diff>
--- a/Matlab/Bifilar Pendulum/Bifilar pendulum test 1.xlsx
+++ b/Matlab/Bifilar Pendulum/Bifilar pendulum test 1.xlsx
@@ -80,7 +80,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,7 +121,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +473,7 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E4">
-        <f>(H4*9.81*F4^2)/(4*(PI()^2)*G4*I4^2)</f>
+        <f t="shared" ref="E4:E12" si="0">(H4*9.81*F4^2)/(4*(PI()^2)*G4*I4^2)</f>
         <v>0.16830762809568864</v>
       </c>
       <c r="F4">
@@ -505,7 +505,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E5">
-        <f>(H5*9.81*F5^2)/(4*(PI()^2)*G5*I5^2)</f>
+        <f t="shared" si="0"/>
         <v>0.17036896357467962</v>
       </c>
       <c r="F5">
@@ -518,7 +518,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I15" si="0">1/L5</f>
+        <f t="shared" ref="I5:I12" si="1">1/L5</f>
         <v>0.29173230643561471</v>
       </c>
       <c r="J5">
@@ -528,7 +528,7 @@
         <v>171.39</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L15" si="1">K5/J5</f>
+        <f t="shared" ref="L5:L12" si="2">K5/J5</f>
         <v>3.4277999999999995</v>
       </c>
       <c r="P5" t="s">
@@ -540,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <f>(H6*9.81*F6^2)/(4*(PI()^2)*G6*I6^2)</f>
+        <f t="shared" si="0"/>
         <v>0.16914848482195632</v>
       </c>
       <c r="F6">
@@ -553,7 +553,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29278290147855363</v>
       </c>
       <c r="J6">
@@ -563,7 +563,7 @@
         <v>68.31</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4155000000000002</v>
       </c>
     </row>
@@ -573,7 +573,7 @@
         <v>0.17019671427704247</v>
       </c>
       <c r="E7">
-        <f>(H7*9.81*F7^2)/(4*(PI()^2)*G7*I7^2)</f>
+        <f t="shared" si="0"/>
         <v>0.170537992723204</v>
       </c>
       <c r="F7">
@@ -586,7 +586,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29158769499927101</v>
       </c>
       <c r="J7">
@@ -596,13 +596,13 @@
         <v>68.59</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4295</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E8">
-        <f>(H8*9.81*F8^2)/(4*(PI()^2)*G8*I8^2)</f>
+        <f t="shared" si="0"/>
         <v>0.16939619436602332</v>
       </c>
       <c r="F8">
@@ -615,7 +615,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29256875365710938</v>
       </c>
       <c r="J8">
@@ -625,13 +625,13 @@
         <v>68.36</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4180000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E9">
-        <f>(H9*9.81*F9^2)/(4*(PI()^2)*G9*I9^2)</f>
+        <f t="shared" si="0"/>
         <v>0.1715506026276486</v>
       </c>
       <c r="F9">
@@ -644,7 +644,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29072584552766739</v>
       </c>
       <c r="J9">
@@ -654,13 +654,13 @@
         <v>103.19</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4396666666666667</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10">
-        <f>(H10*9.81*F10^2)/(4*(PI()^2)*G10*I10^2)</f>
+        <f t="shared" si="0"/>
         <v>0.17118505347896001</v>
       </c>
       <c r="F10">
@@ -673,7 +673,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29103608847497092</v>
       </c>
       <c r="J10">
@@ -683,13 +683,13 @@
         <v>34.36</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4359999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11">
-        <f>(H11*9.81*F11^2)/(4*(PI()^2)*G11*I11^2)</f>
+        <f t="shared" si="0"/>
         <v>0.17019008288328424</v>
       </c>
       <c r="F11">
@@ -702,7 +702,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29188558085230587</v>
       </c>
       <c r="J11">
@@ -712,13 +712,13 @@
         <v>51.39</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4260000000000002</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E12">
-        <f>(H12*9.81*F12^2)/(4*(PI()^2)*G12*I12^2)</f>
+        <f t="shared" si="0"/>
         <v>0.17108542592193751</v>
       </c>
       <c r="F12">
@@ -731,7 +731,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29112081513828236</v>
       </c>
       <c r="J12">
@@ -741,7 +741,7 @@
         <v>68.7</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4350000000000001</v>
       </c>
     </row>
@@ -824,7 +824,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I24" si="2">1/L17</f>
+        <f t="shared" ref="I17:I19" si="3">1/L17</f>
         <v>0.3103180760279286</v>
       </c>
       <c r="J17">
@@ -834,7 +834,7 @@
         <v>64.45</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L24" si="3">K17/J17</f>
+        <f t="shared" ref="L17:L19" si="4">K17/J17</f>
         <v>3.2225000000000001</v>
       </c>
     </row>
@@ -853,7 +853,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.31041440322830977</v>
       </c>
       <c r="J18">
@@ -863,7 +863,7 @@
         <v>64.430000000000007</v>
       </c>
       <c r="L18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2215000000000003</v>
       </c>
     </row>
@@ -882,7 +882,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.31167212092878294</v>
       </c>
       <c r="J19">
@@ -892,7 +892,7 @@
         <v>64.17</v>
       </c>
       <c r="L19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2084999999999999</v>
       </c>
     </row>
@@ -930,7 +930,7 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E23">
-        <f>(H23*9.81*F23^2)/(4*(PI()^2)*G23*I23^2)</f>
+        <f t="shared" ref="E23:E30" si="5">(H23*9.81*F23^2)/(4*(PI()^2)*G23*I23^2)</f>
         <v>2.4978508897662382E-2</v>
       </c>
       <c r="F23">
@@ -960,11 +960,11 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E24">
-        <f>(H24*9.81*F24^2)/(4*(PI()^2)*G24*I24^2)</f>
+        <f t="shared" si="5"/>
         <v>2.5246912708039273E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F31" si="4">0.153/2</f>
+        <f t="shared" ref="F24:F30" si="6">0.153/2</f>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G24">
@@ -974,7 +974,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I31" si="5">1/L24</f>
+        <f t="shared" ref="I24:I30" si="7">1/L24</f>
         <v>0.33311125916055967</v>
       </c>
       <c r="J24">
@@ -984,7 +984,7 @@
         <v>60.04</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L31" si="6">K24/J24</f>
+        <f t="shared" ref="L24:L30" si="8">K24/J24</f>
         <v>3.0019999999999998</v>
       </c>
     </row>
@@ -993,11 +993,11 @@
         <v>15</v>
       </c>
       <c r="E25">
-        <f>(H25*9.81*F25^2)/(4*(PI()^2)*G25*I25^2)</f>
+        <f t="shared" si="5"/>
         <v>2.5011980932632148E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G25">
@@ -1007,7 +1007,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.33467202141900937</v>
       </c>
       <c r="J25">
@@ -1017,7 +1017,7 @@
         <v>59.76</v>
       </c>
       <c r="L25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.988</v>
       </c>
     </row>
@@ -1027,11 +1027,11 @@
         <v>2.502757822055849E-2</v>
       </c>
       <c r="E26">
-        <f>(H26*9.81*F26^2)/(4*(PI()^2)*G26*I26^2)</f>
+        <f t="shared" si="5"/>
         <v>2.5082345156503094E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G26">
@@ -1041,7 +1041,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.3342022592072722</v>
       </c>
       <c r="J26">
@@ -1051,17 +1051,17 @@
         <v>149.61000000000001</v>
       </c>
       <c r="L26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9922000000000004</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E27">
-        <f>(H27*9.81*F27^2)/(4*(PI()^2)*G27*I27^2)</f>
+        <f t="shared" si="5"/>
         <v>2.5112531508388328E-2</v>
       </c>
       <c r="F27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G27">
@@ -1071,7 +1071,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.33400133600534399</v>
       </c>
       <c r="J27">
@@ -1081,17 +1081,17 @@
         <v>59.88</v>
       </c>
       <c r="L27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9940000000000002</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E28">
-        <f>(H28*9.81*F28^2)/(4*(PI()^2)*G28*I28^2)</f>
+        <f t="shared" si="5"/>
         <v>2.4894926861897159E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G28">
@@ -1101,7 +1101,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.33545790003354581</v>
       </c>
       <c r="J28">
@@ -1111,17 +1111,17 @@
         <v>59.62</v>
       </c>
       <c r="L28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9809999999999999</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E29">
-        <f>(H29*9.81*F29^2)/(4*(PI()^2)*G29*I29^2)</f>
+        <f t="shared" si="5"/>
         <v>2.4786479625731626E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G29">
@@ -1131,7 +1131,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.33619095646327113</v>
       </c>
       <c r="J29">
@@ -1141,17 +1141,17 @@
         <v>59.49</v>
       </c>
       <c r="L29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9744999999999999</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E30">
-        <f>(H30*9.81*F30^2)/(4*(PI()^2)*G30*I30^2)</f>
+        <f t="shared" si="5"/>
         <v>2.5106940073613915E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6499999999999999E-2</v>
       </c>
       <c r="G30">
@@ -1161,7 +1161,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.33403852577663956</v>
       </c>
       <c r="J30">
@@ -1171,7 +1171,7 @@
         <v>89.81</v>
       </c>
       <c r="L30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9936666666666669</v>
       </c>
     </row>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E35">
-        <f>(H35*9.81*F35^2)/(4*(PI()^2)*G35*I35^2)</f>
+        <f t="shared" ref="E35:E42" si="9">(H35*9.81*F35^2)/(4*(PI()^2)*G35*I35^2)</f>
         <v>0.16955682249590096</v>
       </c>
       <c r="F35">
@@ -1233,11 +1233,11 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E36">
-        <f>(H36*9.81*F36^2)/(4*(PI()^2)*G36*I36^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16961540652327634</v>
       </c>
       <c r="F36">
-        <f t="shared" ref="F36:F42" si="7">0.39/2</f>
+        <f t="shared" ref="F36:F42" si="10">0.39/2</f>
         <v>0.19500000000000001</v>
       </c>
       <c r="G36">
@@ -1247,7 +1247,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I36">
-        <f t="shared" ref="I36:I42" si="8">1/L36</f>
+        <f t="shared" ref="I36:I42" si="11">1/L36</f>
         <v>0.34542314335060448</v>
       </c>
       <c r="J36">
@@ -1257,7 +1257,7 @@
         <v>57.9</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36:L42" si="9">K36/J36</f>
+        <f t="shared" ref="L36:L42" si="12">K36/J36</f>
         <v>2.895</v>
       </c>
     </row>
@@ -1266,11 +1266,11 @@
         <v>14</v>
       </c>
       <c r="E37">
-        <f>(H37*9.81*F37^2)/(4*(PI()^2)*G37*I37^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16973260493506678</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G37">
@@ -1280,7 +1280,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.34530386740331492</v>
       </c>
       <c r="J37">
@@ -1290,7 +1290,7 @@
         <v>57.92</v>
       </c>
       <c r="L37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.8959999999999999</v>
       </c>
     </row>
@@ -1300,11 +1300,11 @@
         <v>0.16926002422188791</v>
       </c>
       <c r="E38">
-        <f>(H38*9.81*F38^2)/(4*(PI()^2)*G38*I38^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16881953074802961</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G38">
@@ -1314,7 +1314,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.34623641022089885</v>
       </c>
       <c r="J38">
@@ -1324,17 +1324,17 @@
         <v>144.41</v>
       </c>
       <c r="L38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.8881999999999999</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E39">
-        <f>(H39*9.81*F39^2)/(4*(PI()^2)*G39*I39^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16838726694118306</v>
       </c>
       <c r="F39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G39">
@@ -1344,7 +1344,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.34668053388802217</v>
       </c>
       <c r="J39">
@@ -1354,17 +1354,17 @@
         <v>57.69</v>
       </c>
       <c r="L39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.8845000000000001</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E40">
-        <f>(H40*9.81*F40^2)/(4*(PI()^2)*G40*I40^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16990847844535206</v>
       </c>
       <c r="F40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G40">
@@ -1374,7 +1374,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.34512510785159622</v>
       </c>
       <c r="J40">
@@ -1384,17 +1384,17 @@
         <v>57.95</v>
       </c>
       <c r="L40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.8975</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E41">
-        <f>(H41*9.81*F41^2)/(4*(PI()^2)*G41*I41^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16891306604964884</v>
       </c>
       <c r="F41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G41">
@@ -1404,7 +1404,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.3461405330564209</v>
       </c>
       <c r="J41">
@@ -1414,17 +1414,17 @@
         <v>57.78</v>
       </c>
       <c r="L41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.8890000000000002</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E42">
-        <f>(H42*9.81*F42^2)/(4*(PI()^2)*G42*I42^2)</f>
+        <f t="shared" si="9"/>
         <v>0.16914701763664552</v>
       </c>
       <c r="F42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="G42">
@@ -1434,7 +1434,7 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="I42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.34590107229332412</v>
       </c>
       <c r="J42">
@@ -1444,7 +1444,7 @@
         <v>86.73</v>
       </c>
       <c r="L42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.891</v>
       </c>
     </row>

</xml_diff>